<commit_message>
Unit tests based on use case
</commit_message>
<xml_diff>
--- a/Pollux/UnitTests/data/Ranges.xlsx
+++ b/Pollux/UnitTests/data/Ranges.xlsx
@@ -12,7 +12,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="data">Table1[]</definedName>
+    <definedName name="checksums">Standard!$D$31:$I$31</definedName>
+    <definedName name="data">Standard!$B$3:$I$30</definedName>
     <definedName name="Header">Table1[#Headers]</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,13 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>D</t>
   </si>
@@ -43,16 +38,189 @@
     <t>H</t>
   </si>
   <si>
-    <t>SUM</t>
+    <t>UnitID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Name3</t>
+  </si>
+  <si>
+    <t>Name4</t>
+  </si>
+  <si>
+    <t>Name5</t>
+  </si>
+  <si>
+    <t>Name6</t>
+  </si>
+  <si>
+    <t>Name7</t>
+  </si>
+  <si>
+    <t>Name8</t>
+  </si>
+  <si>
+    <t>Name9</t>
+  </si>
+  <si>
+    <t>Name10</t>
+  </si>
+  <si>
+    <t>Name11</t>
+  </si>
+  <si>
+    <t>Name12</t>
+  </si>
+  <si>
+    <t>Name13</t>
+  </si>
+  <si>
+    <t>Name14</t>
+  </si>
+  <si>
+    <t>Name15</t>
+  </si>
+  <si>
+    <t>Name16</t>
+  </si>
+  <si>
+    <t>Name17</t>
+  </si>
+  <si>
+    <t>Name18</t>
+  </si>
+  <si>
+    <t>Name19</t>
+  </si>
+  <si>
+    <t>Name20</t>
+  </si>
+  <si>
+    <t>Name21</t>
+  </si>
+  <si>
+    <t>Name22</t>
+  </si>
+  <si>
+    <t>Name23</t>
+  </si>
+  <si>
+    <t>Name24</t>
+  </si>
+  <si>
+    <t>Name25</t>
+  </si>
+  <si>
+    <t>Name26</t>
+  </si>
+  <si>
+    <t>Name27</t>
+  </si>
+  <si>
+    <t>Name28</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -91,17 +259,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <b val="0"/>
@@ -153,6 +326,9 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -164,17 +340,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:I31" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:I31" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B2:I31"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="B"/>
-    <tableColumn id="2" name="C"/>
+    <tableColumn id="1" name="UnitID"/>
+    <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="D" dataDxfId="2" dataCellStyle="Comma"/>
     <tableColumn id="4" name="E" dataDxfId="1" dataCellStyle="Comma"/>
     <tableColumn id="5" name="F"/>
     <tableColumn id="6" name="G"/>
     <tableColumn id="7" name="H"/>
-    <tableColumn id="8" name="SUM" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="I" dataDxfId="0" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -470,51 +646,52 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
-        <v>0.55579354857312491</v>
-      </c>
-      <c r="C3" s="1">
-        <v>556</v>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>506.39865461372602</v>
@@ -532,15 +709,16 @@
         <v>0.82657146479485766</v>
       </c>
       <c r="I3" s="2">
-        <v>1473252699.1865404</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>1473252142.6307468</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
-        <v>0.36961928815449097</v>
-      </c>
-      <c r="C4" s="1">
-        <v>370</v>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="D4" s="2">
         <v>266.01163180258084</v>
@@ -558,15 +736,16 @@
         <v>0.80146980654886113</v>
       </c>
       <c r="I4" s="2">
-        <v>4977471.9994074302</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>4977101.6297881417</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
-        <v>0.59836805206328536</v>
-      </c>
-      <c r="C5" s="1">
-        <v>598</v>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D5" s="2">
         <v>193.84150245721216</v>
@@ -584,15 +763,16 @@
         <v>0.33662368742760251</v>
       </c>
       <c r="I5" s="2">
-        <v>7824012.5134212524</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>7823413.9150532</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
-        <v>0.16463158500855479</v>
-      </c>
-      <c r="C6" s="1">
-        <v>165</v>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D6" s="2">
         <v>180.95428800341051</v>
@@ -610,15 +790,16 @@
         <v>0.56855771865055382</v>
       </c>
       <c r="I6" s="2">
-        <v>7197049.1674303319</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>7196884.0027987463</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
-        <v>0.5203666062767911</v>
-      </c>
-      <c r="C7" s="1">
-        <v>520</v>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D7" s="2">
         <v>375.39649840622707</v>
@@ -636,15 +817,16 @@
         <v>0.47793809018644517</v>
       </c>
       <c r="I7" s="2">
-        <v>4380179.0963612348</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>4379658.5759946285</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
-        <v>0.73729933370447653</v>
-      </c>
-      <c r="C8" s="1">
-        <v>737</v>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="D8" s="2">
         <v>376.29776521483194</v>
@@ -662,15 +844,16 @@
         <v>0.36685023404568451</v>
       </c>
       <c r="I8" s="2">
-        <v>7994130.7279207325</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>7993392.9906213991</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
-        <v>3.8224659317707133E-3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4</v>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D9" s="2">
         <v>510.55808879684315</v>
@@ -688,15 +871,16 @@
         <v>0.47851624071146126</v>
       </c>
       <c r="I9" s="2">
-        <v>719815.30200906086</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>719811.29818659485</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
-        <v>0.80568480151344346</v>
-      </c>
-      <c r="C10" s="1">
-        <v>806</v>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="D10" s="2">
         <v>666.72994368537809</v>
@@ -714,15 +898,16 @@
         <v>0.32422129399420274</v>
       </c>
       <c r="I10" s="2">
-        <v>7668577.4341844218</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>7667770.6284996197</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
-        <v>0.11328217902052029</v>
-      </c>
-      <c r="C11" s="1">
-        <v>113</v>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="2">
         <v>472.64252680416729</v>
@@ -740,15 +925,16 @@
         <v>0.34278402138064046</v>
       </c>
       <c r="I11" s="2">
-        <v>3014968.075413235</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>3014854.962131056</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
-        <v>0.19611161425759904</v>
-      </c>
-      <c r="C12" s="1">
-        <v>196</v>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="D12" s="2">
         <v>315.89308706744634</v>
@@ -766,15 +952,16 @@
         <v>0.95824939280631982</v>
       </c>
       <c r="I12" s="2">
-        <v>332669.7003698828</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>332473.50425826857</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <v>0.18192939397463226</v>
-      </c>
-      <c r="C13" s="1">
-        <v>182</v>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="D13" s="2">
         <v>272.62714239154968</v>
@@ -792,15 +979,16 @@
         <v>0.69893707801259841</v>
       </c>
       <c r="I13" s="2">
-        <v>7596447.7206011191</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>7596265.5386717245</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
-        <v>0.57878966899586981</v>
-      </c>
-      <c r="C14" s="1">
-        <v>579</v>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D14" s="2">
         <v>724.67716088890097</v>
@@ -818,15 +1006,16 @@
         <v>0.716776192068034</v>
       </c>
       <c r="I14" s="2">
-        <v>5693153.6931245765</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>5692574.1143349074</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
-        <v>0.73044638408173057</v>
-      </c>
-      <c r="C15" s="1">
-        <v>730</v>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="D15" s="2">
         <v>495.50622971476065</v>
@@ -844,15 +1033,16 @@
         <v>0.11232053176873924</v>
       </c>
       <c r="I15" s="2">
-        <v>7119871.3743732767</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>7119140.6439268924</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="1">
-        <v>0.2704508274681543</v>
-      </c>
-      <c r="C16" s="1">
-        <v>270</v>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="D16" s="2">
         <v>697.70863498339702</v>
@@ -870,15 +1060,16 @@
         <v>0.77444568319689722</v>
       </c>
       <c r="I16" s="2">
-        <v>9425186.6119501125</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>9424916.3414992858</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="1">
-        <v>0.67209376640413065</v>
-      </c>
-      <c r="C17" s="1">
-        <v>672</v>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="D17" s="2">
         <v>269.89309098983091</v>
@@ -896,15 +1087,16 @@
         <v>0.12371503503090919</v>
       </c>
       <c r="I17" s="2">
-        <v>2951238.4965112982</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>2950565.824417532</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
-        <v>0.21117435429332987</v>
-      </c>
-      <c r="C18" s="1">
-        <v>211</v>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="D18" s="2">
         <v>78.148686175574014</v>
@@ -922,15 +1114,16 @@
         <v>0.86224531315748809</v>
       </c>
       <c r="I18" s="2">
-        <v>3469163.0363526382</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>3468951.8251782842</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
-        <v>0.85333012486346804</v>
-      </c>
-      <c r="C19" s="1">
-        <v>853</v>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="D19" s="2">
         <v>450.75617774060095</v>
@@ -948,15 +1141,16 @@
         <v>0.99400578781173443</v>
       </c>
       <c r="I19" s="2">
-        <v>1668634.8223151038</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>1667780.968984979</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
-        <v>0.66568579281453899</v>
-      </c>
-      <c r="C20" s="1">
-        <v>666</v>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D20" s="2">
         <v>553.59966326934443</v>
@@ -974,15 +1168,16 @@
         <v>0.41739116082476535</v>
       </c>
       <c r="I20" s="2">
-        <v>759136.0918392461</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>758469.4261534533</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="1">
-        <v>0.57581573816933496</v>
-      </c>
-      <c r="C21" s="1">
-        <v>576</v>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D21" s="2">
         <v>628.0380875105061</v>
@@ -1000,15 +1195,16 @@
         <v>0.67210493422894424</v>
       </c>
       <c r="I21" s="2">
-        <v>8177328.2302024057</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>8176751.6543866675</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="1">
-        <v>0.60492463456133772</v>
-      </c>
-      <c r="C22" s="1">
-        <v>605</v>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D22" s="2">
         <v>212.87579587990291</v>
@@ -1026,15 +1222,16 @@
         <v>0.98683478642802647</v>
       </c>
       <c r="I22" s="2">
-        <v>472857.9532838572</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>472252.34835922264</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="1">
-        <v>0.84910973388123656</v>
-      </c>
-      <c r="C23" s="1">
-        <v>849</v>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D23" s="2">
         <v>581.31436090493253</v>
@@ -1052,15 +1249,16 @@
         <v>0.26484018283948374</v>
       </c>
       <c r="I23" s="2">
-        <v>2082448.5828096445</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>2081598.7336999106</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="1">
-        <v>0.72992452623432058</v>
-      </c>
-      <c r="C24" s="1">
-        <v>730</v>
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D24" s="2">
         <v>185.56077015332608</v>
@@ -1078,15 +1276,16 @@
         <v>5.3502946434212717E-2</v>
       </c>
       <c r="I24" s="2">
-        <v>1305612.3947714679</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>1304881.6648469416</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="1">
-        <v>0.31071132265338608</v>
-      </c>
-      <c r="C25" s="1">
-        <v>311</v>
+      <c r="B25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D25" s="2">
         <v>130.92615956498946</v>
@@ -1104,15 +1303,16 @@
         <v>0.94983369868301193</v>
       </c>
       <c r="I25" s="2">
-        <v>1036179.8693468414</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>1035868.5586355188</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="1">
-        <v>0.10620717816592085</v>
-      </c>
-      <c r="C26" s="1">
-        <v>106</v>
+      <c r="B26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D26" s="2">
         <v>3.2731603406598806</v>
@@ -1130,15 +1330,16 @@
         <v>0.34097468200677994</v>
       </c>
       <c r="I26" s="2">
-        <v>5835769.9037882676</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>5835663.7975810887</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="1">
-        <v>0.62258894060591652</v>
-      </c>
-      <c r="C27" s="1">
-        <v>623</v>
+      <c r="B27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D27" s="2">
         <v>554.18308930753108</v>
@@ -1156,15 +1357,16 @@
         <v>0.19922970872351364</v>
       </c>
       <c r="I27" s="2">
-        <v>2434518.3749125167</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>2433894.7523235762</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="1">
-        <v>0.16821415343618995</v>
-      </c>
-      <c r="C28" s="1">
-        <v>168</v>
+      <c r="B28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="D28" s="2">
         <v>644.7522713874057</v>
@@ -1182,15 +1384,16 @@
         <v>0.63180596346826967</v>
       </c>
       <c r="I28" s="2">
-        <v>3249745.3033126029</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>3249577.1350984494</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="1">
-        <v>0.84379597017320129</v>
-      </c>
-      <c r="C29" s="1">
-        <v>844</v>
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D29" s="2">
         <v>226.98957858323823</v>
@@ -1208,15 +1411,16 @@
         <v>0.41643960340795905</v>
       </c>
       <c r="I29" s="2">
-        <v>7837939.6881791363</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>7837094.8443831662</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="1">
-        <v>0.32710864612415846</v>
-      </c>
-      <c r="C30" s="1">
-        <v>327</v>
+      <c r="B30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D30" s="2">
         <v>565.80815444010136</v>
@@ -1234,33 +1438,36 @@
         <v>0.24549017856998789</v>
       </c>
       <c r="I30" s="2">
-        <v>9245323.1966021229</v>
+        <f>SUM(Table1[[#This Row],[D]:[H]])</f>
+        <v>9244995.869493477</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="1">
-        <v>13.367280631404912</v>
-      </c>
-      <c r="C31" s="3">
-        <v>13367</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1">
+        <f t="shared" ref="D31:G31" si="0">SUM(D3:D30)</f>
         <v>11141.362201078375</v>
       </c>
       <c r="E31" s="2">
+        <f t="shared" si="0"/>
         <v>1597697566.1982722</v>
       </c>
       <c r="F31" s="1">
+        <f t="shared" si="0"/>
         <v>12.488113967731763</v>
       </c>
       <c r="G31" s="1">
+        <f t="shared" si="0"/>
         <v>13.188791742120877</v>
       </c>
       <c r="H31" s="1">
+        <f>SUM(H3:H30)</f>
         <v>14.942675417207983</v>
       </c>
       <c r="I31" s="2">
-        <v>1597722128.5473349</v>
+        <f>SUM(I3:I30)</f>
+        <v>1597708748.1800535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>